<commit_message>
Convert parameters from rds to csv, update trade_parameters spreadsheet
</commit_message>
<xml_diff>
--- a/literature_review/message/trade_parameters.xlsx
+++ b/literature_review/message/trade_parameters.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\message_trade\literature_review\message\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D62A7CB-4744-4DCE-8743-08ACE4199BD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1CEDFC5-594A-4E12-99F1-8C32780824CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="8385" activeTab="2" xr2:uid="{45DE8BD4-7907-4C55-857A-1C652EFA390E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1" xr2:uid="{45DE8BD4-7907-4C55-857A-1C652EFA390E}"/>
   </bookViews>
   <sheets>
     <sheet name="Global Pool Parameters" sheetId="1" r:id="rId1"/>
     <sheet name="Bilateral Trade Parameters" sheetId="2" r:id="rId2"/>
     <sheet name="Cost parameters" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="106">
   <si>
     <t>Segment</t>
   </si>
@@ -287,6 +288,69 @@
   </si>
   <si>
     <t>Index of level-2 embodied conflict</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>AFR</t>
+  </si>
+  <si>
+    <t>WEU</t>
+  </si>
+  <si>
+    <t>PAO</t>
+  </si>
+  <si>
+    <t>eff_distance</t>
+  </si>
+  <si>
+    <t>eff_dispute</t>
+  </si>
+  <si>
+    <t>eff_war</t>
+  </si>
+  <si>
+    <t>eff_embedded_dispute</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>commodity</t>
+  </si>
+  <si>
+    <t>crudeoil</t>
+  </si>
+  <si>
+    <t>lng</t>
+  </si>
+  <si>
+    <t>scenario</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>dispute</t>
+  </si>
+  <si>
+    <t>war</t>
+  </si>
+  <si>
+    <t>embedded_dispute</t>
+  </si>
+  <si>
+    <t>No conflict</t>
+  </si>
+  <si>
+    <t>Disputes, no conflict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">change the commodity (e.g. gas_exp_weu- gas_weu) + change level too (e.g. "shipped oil") &lt;- remember to change the import level/commodity too </t>
+  </si>
+  <si>
+    <t>check in gdx file</t>
   </si>
 </sst>
 </file>
@@ -310,7 +374,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,6 +384,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -336,13 +418,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E31A98C1-91C5-40AB-A3BC-2A8CBE5FB08A}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C12"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,7 +966,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B13" t="s">
@@ -896,7 +986,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B14" t="s">
@@ -955,8 +1045,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B17" t="s">
@@ -975,7 +1065,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -995,7 +1085,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -1015,7 +1105,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1035,8 +1125,8 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B21" t="s">
@@ -1054,8 +1144,11 @@
       <c r="F21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1075,7 +1168,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -1095,8 +1188,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B24" t="s">
@@ -1114,8 +1207,11 @@
       <c r="F24" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1135,7 +1231,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1155,7 +1251,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1175,8 +1271,8 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B28" t="s">
@@ -1208,8 +1304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3FFD0B9-5379-481E-888E-01E463344E65}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,7 +1327,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1251,63 +1347,63 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C4" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C5" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C6" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="8" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1331,243 +1427,243 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="C8" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="C9" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C10" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="C10" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="C11" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D12" t="s">
-        <v>73</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="D12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" t="s">
-        <v>73</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="C13" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C14" t="s">
-        <v>73</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="C14" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="C15" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D16" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="D16" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D17" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D17" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D18" t="s">
-        <v>73</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D18" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="C19" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="8" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1631,83 +1727,83 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D23" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="D23" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D24" t="s">
-        <v>73</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="D24" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D25" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="D25" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C26" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="C26" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="8" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1723,8 +1819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD9A031-B1B8-4DD1-9BCD-F65EF312A3FA}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1851,4 +1947,528 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B0652A9-5D21-4437-BEB6-BBAAA2D75CD2}">
+  <dimension ref="A2:H27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="2">
+        <f ca="1">RAND()</f>
+        <v>0.50974471180367309</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" ref="D3:G8" ca="1" si="0">RAND()</f>
+        <v>0.79099584639338971</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.29692979597798852</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.56025872137423438</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" ref="C4:C8" ca="1" si="1">RAND()</f>
+        <v>0.52733140628565145</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.70294402053208838</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.13209443174687263</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.20439859588664222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.10580331382252584</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.15303456175959396</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.74947638716942178</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.61644667717074353</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.39678185579140968</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.70590518657275025</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.55002466019500307</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.2149562571752055</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.90248447051473368</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.74899993324995362</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>6.4110177820800862E-2</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.23393777875757837</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.10244523317139953</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.65008006190019962</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.60070757781335415</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.10794190415786065</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16">
+        <f ca="1">RANDBETWEEN(100,100000)</f>
+        <v>6261</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ref="D17:D27" ca="1" si="2">RANDBETWEEN(100,100000)</f>
+        <v>63593</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ca="1" si="2"/>
+        <v>90024</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ca="1" si="2"/>
+        <v>87508</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ca="1" si="2"/>
+        <v>56148</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ca="1" si="2"/>
+        <v>44346</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22">
+        <f t="shared" ca="1" si="2"/>
+        <v>33123</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ref="E17:H27" ca="1" si="3">RANDBETWEEN(0,10)</f>
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f t="shared" ca="1" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ca="1" si="2"/>
+        <v>93937</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ca="1" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24">
+        <f t="shared" ca="1" si="2"/>
+        <v>75799</v>
+      </c>
+      <c r="E24">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25">
+        <f t="shared" ca="1" si="2"/>
+        <v>47307</v>
+      </c>
+      <c r="E25">
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <f t="shared" ca="1" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D26">
+        <f t="shared" ca="1" si="2"/>
+        <v>63280</v>
+      </c>
+      <c r="E26">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27">
+        <f t="shared" ca="1" si="2"/>
+        <v>73233</v>
+      </c>
+      <c r="E27">
+        <f t="shared" ca="1" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>